<commit_message>
Updates to manuscript revision, figures, response letter. Still work in progress.
</commit_message>
<xml_diff>
--- a/data/PostReviewMitoWesterns.xlsx
+++ b/data/PostReviewMitoWesterns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Stephenson\Mouse Work\Maternal MCP230 exposure\Western blots\Quads\Post review blots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Stephenson\Mouse Work\Maternal MCP230 exposure\Western blots\Quads\Post review blots\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t>NDUFB8</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>PGC1a</t>
+  </si>
+  <si>
+    <t>SLN</t>
   </si>
 </sst>
 </file>
@@ -371,15 +374,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -404,8 +407,11 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>276</v>
       </c>
@@ -413,7 +419,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>0.91711607701556164</v>
+        <v>0.79560981542308729</v>
       </c>
       <c r="D2">
         <v>0.94807260303478358</v>
@@ -430,14 +436,20 @@
       <c r="H2">
         <v>0.81697518092403698</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>0.43976474573583102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>277</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3">
+        <v>0.79440269061915325</v>
+      </c>
       <c r="D3">
         <v>0.79908149104394566</v>
       </c>
@@ -453,14 +465,20 @@
       <c r="H3">
         <v>0.63764816171992356</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>0.4039177700424238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>278</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4">
+        <v>0.7774253599701495</v>
+      </c>
       <c r="D4">
         <v>2.2377781571257396</v>
       </c>
@@ -476,8 +494,11 @@
       <c r="H4">
         <v>1.3064664697413189</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1.1265785295055808</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>279</v>
       </c>
@@ -485,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>1.3284969662590127</v>
+        <v>1.4333901404847211</v>
       </c>
       <c r="D5">
         <v>1.5784156777048168</v>
@@ -502,8 +523,11 @@
       <c r="H5">
         <v>1.139059638918668</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1.4567495204272489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>280</v>
       </c>
@@ -511,7 +535,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>1.2180058311419888</v>
+        <v>1.1991719935028888</v>
       </c>
       <c r="D6">
         <v>2.49782695808008</v>
@@ -528,8 +552,11 @@
       <c r="H6">
         <v>1.7448213697667971</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1.5729894342889159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>281</v>
       </c>
@@ -537,7 +564,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>0.74357062015009956</v>
+        <v>0.82551794543448231</v>
       </c>
       <c r="D7">
         <v>0.46118505164707257</v>
@@ -555,7 +582,7 @@
         <v>0.76653180222738315</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>290</v>
       </c>
@@ -563,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0.93459241169684248</v>
+        <v>1.0338528611826157</v>
       </c>
       <c r="D8">
         <v>0.49363660865377401</v>
@@ -580,8 +607,11 @@
       <c r="H8">
         <v>0.82559223971498419</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>0.57369757586764669</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>291</v>
       </c>
@@ -589,7 +619,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.98209253015889331</v>
+        <v>0.42272274660492465</v>
       </c>
       <c r="D9">
         <v>0.4721943952419777</v>
@@ -606,8 +636,11 @@
       <c r="H9">
         <v>0.91277146659789765</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1.0604473023786718</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>292</v>
       </c>
@@ -615,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>0.7255628930969904</v>
+        <v>0.85735468748372179</v>
       </c>
       <c r="D10">
         <v>0.24857038591089006</v>
@@ -632,8 +665,11 @@
       <c r="H10">
         <v>0.98643527841120537</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1.7238787383873213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>293</v>
       </c>
@@ -641,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>1.1505626704806118</v>
+        <v>1.8605517592942551</v>
       </c>
       <c r="D11">
         <v>0.26323867155691993</v>
@@ -658,8 +694,11 @@
       <c r="H11">
         <v>0.86369839197778664</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>0.64197638336635954</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>201</v>
       </c>
@@ -667,7 +706,7 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>0.74172742862739494</v>
+        <v>0.87573611402298368</v>
       </c>
       <c r="D12">
         <v>1.590126177364805</v>
@@ -684,8 +723,11 @@
       <c r="H12">
         <v>1.2475559035881181</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>0.34245232816823429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>202</v>
       </c>
@@ -693,7 +735,7 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <v>1.2243649442529405</v>
+        <v>0.99277677560930144</v>
       </c>
       <c r="D13">
         <v>1.6023261947066572</v>
@@ -710,8 +752,11 @@
       <c r="H13">
         <v>0.84080087420248995</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>0.5512732208312906</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>203</v>
       </c>
@@ -719,7 +764,7 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>1.8059734517563431</v>
+        <v>1.9465817875503271</v>
       </c>
       <c r="D14">
         <v>1.1456887156957443</v>
@@ -736,8 +781,11 @@
       <c r="H14">
         <v>1.0806570095906716</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>2.7937192411456748</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>204</v>
       </c>
@@ -745,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>0.90896821425060748</v>
+        <v>1.0656741128686928</v>
       </c>
       <c r="D15">
         <v>2.0336523281536758</v>
@@ -762,8 +810,11 @@
       <c r="H15">
         <v>1.1771567021513254</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>2.5572209023274066</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>207</v>
       </c>
@@ -771,7 +822,7 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>0.75179220868708119</v>
+        <v>0.80257646846846287</v>
       </c>
       <c r="D16">
         <v>1.6875786991804342</v>
@@ -788,8 +839,11 @@
       <c r="H16">
         <v>1.7707665655025198</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>1.2215606663616907</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>208</v>
       </c>
@@ -797,7 +851,7 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <v>1.2599458012360847</v>
+        <v>1.8101282205499289</v>
       </c>
       <c r="D17">
         <v>0.50111648705875877</v>
@@ -814,8 +868,11 @@
       <c r="H17">
         <v>0.68785468302005559</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>0.60611960391135367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>209</v>
       </c>
@@ -823,7 +880,7 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>0.94850010499484716</v>
+        <v>1.649148909933007</v>
       </c>
       <c r="D18">
         <v>0.32559529368119011</v>
@@ -840,8 +897,11 @@
       <c r="H18">
         <v>0.66639403263309371</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1.1927796215804063</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>214</v>
       </c>
@@ -849,7 +909,7 @@
         <v>8</v>
       </c>
       <c r="C19">
-        <v>1.0378200538622229</v>
+        <v>0.80609029842317526</v>
       </c>
       <c r="D19">
         <v>0.6513787190742204</v>
@@ -866,8 +926,11 @@
       <c r="H19">
         <v>1.5254205160607481</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1.422975280265582</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>250</v>
       </c>
@@ -875,7 +938,7 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>0.69072401530409588</v>
+        <v>1.0356526980103515</v>
       </c>
       <c r="D20">
         <v>0.217273116138539</v>
@@ -892,8 +955,11 @@
       <c r="H20">
         <v>0.70137292936823259</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1.1447176216445916</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2500</v>
       </c>
@@ -901,7 +967,7 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>1.6571185560467379</v>
+        <v>2.4997768616133427</v>
       </c>
       <c r="D21">
         <v>0.49818339164787584</v>
@@ -917,6 +983,9 @@
       </c>
       <c r="H21">
         <v>1.3288090323132817</v>
+      </c>
+      <c r="I21">
+        <v>0.60384917063911503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>